<commit_message>
finals slides , change management process
</commit_message>
<xml_diff>
--- a/Documentation/Deliverables/MIDTERMS PPT SLIDES/Bug Metrics.xlsx
+++ b/Documentation/Deliverables/MIDTERMS PPT SLIDES/Bug Metrics.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="16925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17329"/>
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Teh Kaixin\Desktop\FYP GIT\Ulink\Documentation\MIDTERMS PPT SLIDES\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Teh Kaixin\Desktop\FYP GIT\Ulink\Documentation\Deliverables\MIDTERMS PPT SLIDES\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1785" yWindow="465" windowWidth="25515" windowHeight="15540" firstSheet="1" activeTab="2"/>
+    <workbookView xWindow="1785" yWindow="465" windowWidth="25515" windowHeight="15540" firstSheet="1" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Overall Bug Score" sheetId="1" state="hidden" r:id="rId1"/>
@@ -1128,7 +1128,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="23">
+  <borders count="24">
     <border>
       <left/>
       <right/>
@@ -1422,11 +1422,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="133">
+  <cellXfs count="134">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1730,24 +1741,25 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1985,10 +1997,10 @@
           <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
-              <c:f>'Bug Log Iter 1-10'!$J$23:$J$29</c:f>
+              <c:f>'Bug Log Iter 1-10'!$J$23:$J$33</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>12</c:v>
                 </c:pt>
@@ -2009,6 +2021,18 @@
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2045,10 +2069,10 @@
           <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
-              <c:f>'Bug Log Iter 1-10'!$K$23:$K$29</c:f>
+              <c:f>'Bug Log Iter 1-10'!$K$23:$K$33</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>5</c:v>
                 </c:pt>
@@ -2068,6 +2092,18 @@
                   <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="6">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="10">
                   <c:v>5</c:v>
                 </c:pt>
               </c:numCache>
@@ -2105,10 +2141,10 @@
           <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
-              <c:f>'Bug Log Iter 1-10'!$L$23:$L$29</c:f>
+              <c:f>'Bug Log Iter 1-10'!$L$23:$L$33</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -2128,6 +2164,18 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="10">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -2441,6 +2489,7 @@
     <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
     <c:pageSetup/>
   </c:printSettings>
+  <c:userShapes r:id="rId3"/>
 </c:chartSpace>
 </file>
 
@@ -3055,7 +3104,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="5" name="Chart 4"/>
+        <xdr:cNvPr id="5" name="Chart 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000005000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -3073,19 +3128,25 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>466725</xdr:colOff>
+      <xdr:colOff>352425</xdr:colOff>
       <xdr:row>9</xdr:row>
-      <xdr:rowOff>323850</xdr:rowOff>
+      <xdr:rowOff>314325</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>676249</xdr:colOff>
+      <xdr:colOff>561949</xdr:colOff>
       <xdr:row>10</xdr:row>
-      <xdr:rowOff>104754</xdr:rowOff>
+      <xdr:rowOff>95229</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="6" name="Picture 5"/>
+        <xdr:cNvPr id="6" name="Picture 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000006000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -3098,7 +3159,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6429375" y="3381375"/>
+          <a:off x="6315075" y="3371850"/>
           <a:ext cx="209524" cy="171429"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -3111,19 +3172,25 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>542925</xdr:colOff>
+      <xdr:colOff>552450</xdr:colOff>
       <xdr:row>9</xdr:row>
-      <xdr:rowOff>323850</xdr:rowOff>
+      <xdr:rowOff>333375</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>761973</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>9490</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>190145</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>161898</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="7" name="Picture 6"/>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4B53664D-88C8-4965-BB84-F6F9DB8080E1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -3136,8 +3203,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7239000" y="3381375"/>
-          <a:ext cx="219048" cy="276190"/>
+          <a:off x="7248525" y="3390900"/>
+          <a:ext cx="2838095" cy="219048"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3148,20 +3215,26 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>561975</xdr:colOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
       <xdr:row>9</xdr:row>
       <xdr:rowOff>314325</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>399923</xdr:colOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>285729</xdr:colOff>
       <xdr:row>10</xdr:row>
-      <xdr:rowOff>133324</xdr:rowOff>
+      <xdr:rowOff>123800</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="8" name="Picture 7"/>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{159A26EC-9AB5-4366-ACCD-71863AC33B97}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -3174,121 +3247,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8048625" y="3371850"/>
-          <a:ext cx="1019048" cy="209524"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>390525</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>342900</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>104775</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>133350</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="10" name="Picture 9"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill rotWithShape="1">
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
-        <a:srcRect r="66960" b="17381"/>
-        <a:stretch/>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="9648825" y="3400425"/>
-          <a:ext cx="352425" cy="180975"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>533400</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>352425</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>152374</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>161900</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="11" name="Picture 10"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="10429875" y="3409950"/>
-          <a:ext cx="209524" cy="200000"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>142875</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>333375</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>371446</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>76158</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="12" name="Picture 11"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="11220450" y="3390900"/>
-          <a:ext cx="228571" cy="333333"/>
+          <a:off x="6810375" y="3371850"/>
+          <a:ext cx="171429" cy="200000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3298,6 +3258,126 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:userShapes xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.76054</cdr:x>
+      <cdr:y>0.80998</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.8012</cdr:x>
+      <cdr:y>0.8361</cdr:y>
+    </cdr:to>
+    <cdr:pic>
+      <cdr:nvPicPr>
+        <cdr:cNvPr id="3" name="chart">
+          <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D4D695AA-7B17-47A4-AB75-D6F4E239D57E}"/>
+            </a:ext>
+          </a:extLst>
+        </cdr:cNvPr>
+        <cdr:cNvPicPr>
+          <a:picLocks xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" noChangeAspect="1"/>
+        </cdr:cNvPicPr>
+      </cdr:nvPicPr>
+      <cdr:blipFill rotWithShape="1">
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:srcRect xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" l="1" t="-1" r="71871" b="47611"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+      </cdr:blipFill>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="4810125" y="3248026"/>
+          <a:ext cx="257175" cy="104776"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </cdr:spPr>
+    </cdr:pic>
+  </cdr:relSizeAnchor>
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.91717</cdr:x>
+      <cdr:y>0.80047</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.96234</cdr:x>
+      <cdr:y>0.85035</cdr:y>
+    </cdr:to>
+    <cdr:pic>
+      <cdr:nvPicPr>
+        <cdr:cNvPr id="4" name="chart">
+          <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{86CB7D55-DCE3-41FD-8B69-ED3EB9C900A5}"/>
+            </a:ext>
+          </a:extLst>
+        </cdr:cNvPr>
+        <cdr:cNvPicPr>
+          <a:picLocks xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" noChangeAspect="1"/>
+        </cdr:cNvPicPr>
+      </cdr:nvPicPr>
+      <cdr:blipFill>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:fillRect/>
+        </a:stretch>
+      </cdr:blipFill>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="5800725" y="3209925"/>
+          <a:ext cx="285714" cy="200000"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </cdr:spPr>
+    </cdr:pic>
+  </cdr:relSizeAnchor>
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.84187</cdr:x>
+      <cdr:y>0.80998</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.87851</cdr:x>
+      <cdr:y>0.8464</cdr:y>
+    </cdr:to>
+    <cdr:pic>
+      <cdr:nvPicPr>
+        <cdr:cNvPr id="6" name="chart">
+          <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6DC78B82-908E-4E20-8C2D-36549E3D604A}"/>
+            </a:ext>
+          </a:extLst>
+        </cdr:cNvPr>
+        <cdr:cNvPicPr>
+          <a:picLocks xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" noChangeAspect="1"/>
+        </cdr:cNvPicPr>
+      </cdr:nvPicPr>
+      <cdr:blipFill rotWithShape="1">
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:srcRect xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" l="39241" t="3173" r="35409" b="23801"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+      </cdr:blipFill>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="5324474" y="3248026"/>
+          <a:ext cx="231775" cy="146050"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </cdr:spPr>
+    </cdr:pic>
+  </cdr:relSizeAnchor>
+</c:userShapes>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -7244,7 +7324,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="L14:M16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A11" workbookViewId="0">
       <selection activeCell="L17" sqref="L17"/>
     </sheetView>
   </sheetViews>
@@ -7284,8 +7364,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R40"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="O1" sqref="O1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7500,7 +7580,7 @@
       <c r="G10" s="63"/>
     </row>
     <row r="11" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="128"/>
+      <c r="A11" s="127"/>
       <c r="B11" s="87" t="s">
         <v>277</v>
       </c>
@@ -7523,12 +7603,12 @@
     </row>
     <row r="12" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="119"/>
-      <c r="B12" s="129" t="s">
+      <c r="B12" s="128" t="s">
         <v>26</v>
       </c>
-      <c r="C12" s="130"/>
-      <c r="D12" s="130"/>
-      <c r="E12" s="131"/>
+      <c r="C12" s="129"/>
+      <c r="D12" s="129"/>
+      <c r="E12" s="130"/>
       <c r="F12" s="71">
         <f>SUM(F3:F10)</f>
         <v>17</v>
@@ -7607,7 +7687,7 @@
       </c>
     </row>
     <row r="16" spans="1:7" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="132"/>
+      <c r="A16" s="131"/>
       <c r="B16" s="89" t="s">
         <v>277</v>
       </c>
@@ -7628,12 +7708,12 @@
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A17" s="123"/>
-      <c r="B17" s="129" t="s">
+      <c r="B17" s="128" t="s">
         <v>41</v>
       </c>
-      <c r="C17" s="130"/>
-      <c r="D17" s="130"/>
-      <c r="E17" s="131"/>
+      <c r="C17" s="129"/>
+      <c r="D17" s="129"/>
+      <c r="E17" s="130"/>
       <c r="F17" s="71">
         <f>SUM(F13:F15)</f>
         <v>12</v>
@@ -7689,12 +7769,12 @@
     </row>
     <row r="20" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A20" s="118"/>
-      <c r="B20" s="127" t="s">
+      <c r="B20" s="132" t="s">
         <v>84</v>
       </c>
-      <c r="C20" s="127"/>
-      <c r="D20" s="127"/>
-      <c r="E20" s="127"/>
+      <c r="C20" s="132"/>
+      <c r="D20" s="132"/>
+      <c r="E20" s="132"/>
       <c r="F20" s="71">
         <f>SUM(F18)</f>
         <v>34</v>
@@ -7788,12 +7868,12 @@
     </row>
     <row r="24" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A24" s="118"/>
-      <c r="B24" s="127" t="s">
+      <c r="B24" s="132" t="s">
         <v>278</v>
       </c>
-      <c r="C24" s="127"/>
-      <c r="D24" s="127"/>
-      <c r="E24" s="127"/>
+      <c r="C24" s="132"/>
+      <c r="D24" s="132"/>
+      <c r="E24" s="132"/>
       <c r="F24" s="71">
         <f>SUM(F22)</f>
         <v>23</v>
@@ -8030,23 +8110,20 @@
     </row>
     <row r="30" spans="1:18" x14ac:dyDescent="0.25">
       <c r="I30" s="92">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="J30" s="91">
-        <f>C31</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="K30" s="4">
-        <f>D31</f>
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="L30" s="90">
-        <f>E31</f>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="M30" s="73">
         <f t="shared" si="2"/>
-        <v>3</v>
+        <v>24</v>
       </c>
     </row>
     <row r="31" spans="1:18" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -8073,15 +8150,13 @@
         <v>68</v>
       </c>
       <c r="I31" s="98">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="J31" s="99">
-        <f>C36</f>
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="K31" s="100">
-        <f>D36</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="L31" s="101">
         <f>E36</f>
@@ -8089,7 +8164,7 @@
       </c>
       <c r="M31" s="102">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="32" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -8110,15 +8185,13 @@
       </c>
       <c r="G32" s="22"/>
       <c r="I32" s="105">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="J32" s="106">
-        <f>C42</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="K32" s="107">
-        <f>D42</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="L32" s="108">
         <f>E42</f>
@@ -8126,10 +8199,10 @@
       </c>
       <c r="M32" s="109">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A33" s="118"/>
       <c r="B33" s="25" t="s">
         <v>277</v>
@@ -8149,8 +8222,20 @@
       <c r="G33" s="64" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I33" s="133">
+        <v>14</v>
+      </c>
+      <c r="J33">
+        <v>5</v>
+      </c>
+      <c r="K33">
+        <v>5</v>
+      </c>
+      <c r="L33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A34" s="118"/>
       <c r="B34" s="118" t="s">
         <v>280</v>
@@ -8164,7 +8249,7 @@
       </c>
       <c r="G34" s="63"/>
     </row>
-    <row r="36" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="118">
         <v>10</v>
       </c>
@@ -8188,7 +8273,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A37" s="118"/>
       <c r="B37" s="25" t="s">
         <v>287</v>
@@ -8210,7 +8295,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A38" s="118"/>
       <c r="B38" s="25" t="s">
         <v>288</v>
@@ -8230,7 +8315,7 @@
       </c>
       <c r="G38" s="64"/>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A39" s="118"/>
       <c r="B39" s="25" t="s">
         <v>285</v>
@@ -8250,7 +8335,7 @@
       <c r="F39" s="64"/>
       <c r="G39" s="64"/>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A40" s="118"/>
       <c r="B40" s="118" t="s">
         <v>281</v>
@@ -8266,12 +8351,6 @@
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="A3:A12"/>
-    <mergeCell ref="B12:E12"/>
-    <mergeCell ref="A13:A17"/>
-    <mergeCell ref="B17:E17"/>
-    <mergeCell ref="A18:A20"/>
-    <mergeCell ref="B20:E20"/>
     <mergeCell ref="A36:A40"/>
     <mergeCell ref="B40:E40"/>
     <mergeCell ref="A22:A24"/>
@@ -8280,6 +8359,12 @@
     <mergeCell ref="B29:E29"/>
     <mergeCell ref="A31:A34"/>
     <mergeCell ref="B34:E34"/>
+    <mergeCell ref="A3:A12"/>
+    <mergeCell ref="B12:E12"/>
+    <mergeCell ref="A13:A17"/>
+    <mergeCell ref="B17:E17"/>
+    <mergeCell ref="A18:A20"/>
+    <mergeCell ref="B20:E20"/>
   </mergeCells>
   <conditionalFormatting sqref="C3:E9 C11:E11 D10:E10">
     <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">

</xml_diff>

<commit_message>
Finals PPT V2 (missing tech comp, workflow)
</commit_message>
<xml_diff>
--- a/Documentation/Deliverables/MIDTERMS PPT SLIDES/Bug Metrics.xlsx
+++ b/Documentation/Deliverables/MIDTERMS PPT SLIDES/Bug Metrics.xlsx
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="568" uniqueCount="292">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="596" uniqueCount="296">
   <si>
     <t>Task</t>
   </si>
@@ -951,6 +951,18 @@
   </si>
   <si>
     <t>Critical Bug</t>
+  </si>
+  <si>
+    <t>Total Score for Iteration 11</t>
+  </si>
+  <si>
+    <t>Export</t>
+  </si>
+  <si>
+    <t>Reports</t>
+  </si>
+  <si>
+    <t>live database</t>
   </si>
 </sst>
 </file>
@@ -1128,7 +1140,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="24">
+  <borders count="23">
     <border>
       <left/>
       <right/>
@@ -1422,22 +1434,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="134">
+  <cellXfs count="131">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1701,11 +1702,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="17" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
@@ -1715,6 +1711,12 @@
     <xf numFmtId="0" fontId="8" fillId="13" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="13" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1741,6 +1743,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1756,10 +1761,7 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2170,9 +2172,6 @@
                   <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="9">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="10">
@@ -3733,7 +3732,7 @@
       <c r="H2" s="1"/>
     </row>
     <row r="3" spans="1:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="119">
+      <c r="A3" s="116">
         <v>2</v>
       </c>
       <c r="B3" s="11" t="s">
@@ -3760,7 +3759,7 @@
       </c>
     </row>
     <row r="4" spans="1:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="119"/>
+      <c r="A4" s="116"/>
       <c r="B4" s="11" t="s">
         <v>12</v>
       </c>
@@ -3785,7 +3784,7 @@
       </c>
     </row>
     <row r="5" spans="1:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="119"/>
+      <c r="A5" s="116"/>
       <c r="B5" s="11" t="s">
         <v>13</v>
       </c>
@@ -3810,7 +3809,7 @@
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A6" s="119"/>
+      <c r="A6" s="116"/>
       <c r="B6" s="11" t="s">
         <v>32</v>
       </c>
@@ -3826,7 +3825,7 @@
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A7" s="119"/>
+      <c r="A7" s="116"/>
       <c r="B7" s="11" t="s">
         <v>14</v>
       </c>
@@ -3849,7 +3848,7 @@
       </c>
     </row>
     <row r="8" spans="1:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="119"/>
+      <c r="A8" s="116"/>
       <c r="B8" s="11" t="s">
         <v>15</v>
       </c>
@@ -3872,7 +3871,7 @@
       </c>
     </row>
     <row r="9" spans="1:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" s="119"/>
+      <c r="A9" s="116"/>
       <c r="B9" s="11" t="s">
         <v>33</v>
       </c>
@@ -3897,7 +3896,7 @@
       </c>
     </row>
     <row r="10" spans="1:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="A10" s="119"/>
+      <c r="A10" s="116"/>
       <c r="B10" s="12" t="s">
         <v>28</v>
       </c>
@@ -3921,14 +3920,14 @@
       <c r="M10" s="9"/>
     </row>
     <row r="11" spans="1:13" ht="51.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="119"/>
-      <c r="B11" s="120" t="s">
+      <c r="A11" s="116"/>
+      <c r="B11" s="117" t="s">
         <v>26</v>
       </c>
-      <c r="C11" s="121"/>
-      <c r="D11" s="121"/>
-      <c r="E11" s="121"/>
-      <c r="F11" s="122"/>
+      <c r="C11" s="118"/>
+      <c r="D11" s="118"/>
+      <c r="E11" s="118"/>
+      <c r="F11" s="119"/>
       <c r="G11" s="13">
         <f>SUM(G3:G10)</f>
         <v>10</v>
@@ -3939,7 +3938,7 @@
       </c>
     </row>
     <row r="12" spans="1:13" ht="45" x14ac:dyDescent="0.25">
-      <c r="A12" s="123">
+      <c r="A12" s="120">
         <v>3</v>
       </c>
       <c r="B12" s="17" t="s">
@@ -3965,7 +3964,7 @@
       </c>
     </row>
     <row r="13" spans="1:13" ht="45" x14ac:dyDescent="0.25">
-      <c r="A13" s="123"/>
+      <c r="A13" s="120"/>
       <c r="B13" s="17" t="s">
         <v>40</v>
       </c>
@@ -3989,7 +3988,7 @@
       </c>
     </row>
     <row r="14" spans="1:13" ht="45" x14ac:dyDescent="0.25">
-      <c r="A14" s="123"/>
+      <c r="A14" s="120"/>
       <c r="B14" s="23" t="s">
         <v>46</v>
       </c>
@@ -4013,14 +4012,14 @@
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A15" s="123"/>
-      <c r="B15" s="120" t="s">
+      <c r="A15" s="120"/>
+      <c r="B15" s="117" t="s">
         <v>41</v>
       </c>
-      <c r="C15" s="121"/>
-      <c r="D15" s="121"/>
-      <c r="E15" s="121"/>
-      <c r="F15" s="122"/>
+      <c r="C15" s="118"/>
+      <c r="D15" s="118"/>
+      <c r="E15" s="118"/>
+      <c r="F15" s="119"/>
       <c r="G15" s="13">
         <f>SUM(G12:G14)</f>
         <v>39</v>
@@ -4028,7 +4027,7 @@
       <c r="H15" s="16"/>
     </row>
     <row r="16" spans="1:13" ht="45" x14ac:dyDescent="0.25">
-      <c r="A16" s="118">
+      <c r="A16" s="115">
         <v>6</v>
       </c>
       <c r="B16" s="25" t="s">
@@ -4052,14 +4051,14 @@
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="118"/>
-      <c r="B17" s="118" t="s">
+      <c r="A17" s="115"/>
+      <c r="B17" s="115" t="s">
         <v>84</v>
       </c>
-      <c r="C17" s="118"/>
-      <c r="D17" s="118"/>
-      <c r="E17" s="118"/>
-      <c r="F17" s="118"/>
+      <c r="C17" s="115"/>
+      <c r="D17" s="115"/>
+      <c r="E17" s="115"/>
+      <c r="F17" s="115"/>
       <c r="G17" s="13">
         <f>SUM(G16)</f>
         <v>19</v>
@@ -4067,7 +4066,7 @@
       <c r="H17" s="20"/>
     </row>
     <row r="20" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A20" s="118">
+      <c r="A20" s="115">
         <v>6</v>
       </c>
       <c r="B20" s="25" t="s">
@@ -4091,14 +4090,14 @@
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" s="118"/>
-      <c r="B21" s="118" t="s">
+      <c r="A21" s="115"/>
+      <c r="B21" s="115" t="s">
         <v>84</v>
       </c>
-      <c r="C21" s="118"/>
-      <c r="D21" s="118"/>
-      <c r="E21" s="118"/>
-      <c r="F21" s="118"/>
+      <c r="C21" s="115"/>
+      <c r="D21" s="115"/>
+      <c r="E21" s="115"/>
+      <c r="F21" s="115"/>
       <c r="G21" s="13">
         <f>SUM(G20)</f>
         <v>19</v>
@@ -4116,7 +4115,7 @@
       <c r="H22" s="63"/>
     </row>
     <row r="23" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A23" s="118">
+      <c r="A23" s="115">
         <v>8</v>
       </c>
       <c r="B23" s="25" t="s">
@@ -4140,7 +4139,7 @@
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A24" s="118"/>
+      <c r="A24" s="115"/>
       <c r="B24" s="25" t="s">
         <v>206</v>
       </c>
@@ -4162,14 +4161,14 @@
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A25" s="118"/>
-      <c r="B25" s="118" t="s">
+      <c r="A25" s="115"/>
+      <c r="B25" s="115" t="s">
         <v>84</v>
       </c>
-      <c r="C25" s="118"/>
-      <c r="D25" s="118"/>
-      <c r="E25" s="118"/>
-      <c r="F25" s="118"/>
+      <c r="C25" s="115"/>
+      <c r="D25" s="115"/>
+      <c r="E25" s="115"/>
+      <c r="F25" s="115"/>
       <c r="G25" s="13">
         <f>SUM(G23:G24)</f>
         <v>26</v>
@@ -4203,7 +4202,7 @@
   <dimension ref="A1:L100"/>
   <sheetViews>
     <sheetView topLeftCell="B1" zoomScale="77" zoomScaleNormal="77" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A40" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A25" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="E32" sqref="E32"/>
     </sheetView>
   </sheetViews>
@@ -5078,10 +5077,10 @@
         <v>87</v>
       </c>
       <c r="D27" s="30"/>
-      <c r="E27" s="124" t="s">
+      <c r="E27" s="121" t="s">
         <v>100</v>
       </c>
-      <c r="F27" s="124"/>
+      <c r="F27" s="121"/>
       <c r="G27" s="4"/>
       <c r="H27" s="4"/>
       <c r="I27" s="4"/>
@@ -5293,7 +5292,7 @@
       </c>
       <c r="J36" s="4"/>
       <c r="K36" s="4"/>
-      <c r="L36" s="125" t="s">
+      <c r="L36" s="122" t="s">
         <v>203</v>
       </c>
     </row>
@@ -5327,7 +5326,7 @@
       </c>
       <c r="J37" s="4"/>
       <c r="K37" s="4"/>
-      <c r="L37" s="125"/>
+      <c r="L37" s="122"/>
     </row>
     <row r="38" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A38" s="4">
@@ -5359,7 +5358,7 @@
       </c>
       <c r="J38" s="4"/>
       <c r="K38" s="4"/>
-      <c r="L38" s="125"/>
+      <c r="L38" s="122"/>
     </row>
     <row r="39" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A39" s="4">
@@ -5391,7 +5390,7 @@
       </c>
       <c r="J39" s="4"/>
       <c r="K39" s="4"/>
-      <c r="L39" s="125"/>
+      <c r="L39" s="122"/>
     </row>
     <row r="40" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A40" s="4">
@@ -5423,7 +5422,7 @@
       </c>
       <c r="J40" s="4"/>
       <c r="K40" s="4"/>
-      <c r="L40" s="125"/>
+      <c r="L40" s="122"/>
     </row>
     <row r="41" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A41" s="4">
@@ -5455,7 +5454,7 @@
       </c>
       <c r="J41" s="4"/>
       <c r="K41" s="4"/>
-      <c r="L41" s="125"/>
+      <c r="L41" s="122"/>
     </row>
     <row r="42" spans="1:12" ht="60" x14ac:dyDescent="0.25">
       <c r="A42" s="4">
@@ -5487,7 +5486,7 @@
       </c>
       <c r="J42" s="4"/>
       <c r="K42" s="4"/>
-      <c r="L42" s="125"/>
+      <c r="L42" s="122"/>
     </row>
     <row r="43" spans="1:12" ht="60" x14ac:dyDescent="0.25">
       <c r="A43" s="4">
@@ -5519,7 +5518,7 @@
       </c>
       <c r="J43" s="4"/>
       <c r="K43" s="4"/>
-      <c r="L43" s="125"/>
+      <c r="L43" s="122"/>
     </row>
     <row r="44" spans="1:12" ht="60" x14ac:dyDescent="0.25">
       <c r="A44" s="4">
@@ -5551,7 +5550,7 @@
       </c>
       <c r="J44" s="4"/>
       <c r="K44" s="4"/>
-      <c r="L44" s="125"/>
+      <c r="L44" s="122"/>
     </row>
     <row r="45" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A45" s="4">
@@ -5581,7 +5580,7 @@
       <c r="K45" s="5">
         <v>42757</v>
       </c>
-      <c r="L45" s="125"/>
+      <c r="L45" s="122"/>
     </row>
     <row r="46" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A46" s="4">
@@ -6466,7 +6465,7 @@
       <c r="D74" s="30">
         <v>2</v>
       </c>
-      <c r="E74" s="126" t="s">
+      <c r="E74" s="123" t="s">
         <v>229</v>
       </c>
       <c r="F74" s="27" t="s">
@@ -6500,7 +6499,7 @@
       <c r="D75" s="30">
         <v>3</v>
       </c>
-      <c r="E75" s="126"/>
+      <c r="E75" s="123"/>
       <c r="F75" s="27" t="s">
         <v>223</v>
       </c>
@@ -7362,10 +7361,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R40"/>
+  <dimension ref="A1:R65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="O1" sqref="O1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D56" sqref="D56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7418,7 +7417,7 @@
       <c r="G2" s="1"/>
     </row>
     <row r="3" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="119">
+      <c r="A3" s="116">
         <v>2</v>
       </c>
       <c r="B3" s="12" t="s">
@@ -7442,7 +7441,7 @@
       </c>
     </row>
     <row r="4" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="119"/>
+      <c r="A4" s="116"/>
       <c r="B4" s="12" t="s">
         <v>12</v>
       </c>
@@ -7462,7 +7461,7 @@
       </c>
     </row>
     <row r="5" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="119"/>
+      <c r="A5" s="116"/>
       <c r="B5" s="12" t="s">
         <v>13</v>
       </c>
@@ -7484,7 +7483,7 @@
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="119"/>
+      <c r="A6" s="116"/>
       <c r="B6" s="12" t="s">
         <v>32</v>
       </c>
@@ -7502,7 +7501,7 @@
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="119"/>
+      <c r="A7" s="116"/>
       <c r="B7" s="12" t="s">
         <v>14</v>
       </c>
@@ -7522,7 +7521,7 @@
       </c>
     </row>
     <row r="8" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="119"/>
+      <c r="A8" s="116"/>
       <c r="B8" s="12" t="s">
         <v>15</v>
       </c>
@@ -7542,7 +7541,7 @@
       </c>
     </row>
     <row r="9" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" s="119"/>
+      <c r="A9" s="116"/>
       <c r="B9" s="12" t="s">
         <v>33</v>
       </c>
@@ -7564,7 +7563,7 @@
       </c>
     </row>
     <row r="10" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="119"/>
+      <c r="A10" s="116"/>
       <c r="B10" s="86" t="s">
         <v>28</v>
       </c>
@@ -7580,7 +7579,7 @@
       <c r="G10" s="63"/>
     </row>
     <row r="11" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="127"/>
+      <c r="A11" s="125"/>
       <c r="B11" s="87" t="s">
         <v>277</v>
       </c>
@@ -7602,13 +7601,13 @@
       </c>
     </row>
     <row r="12" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="119"/>
-      <c r="B12" s="128" t="s">
+      <c r="A12" s="116"/>
+      <c r="B12" s="126" t="s">
         <v>26</v>
       </c>
-      <c r="C12" s="129"/>
-      <c r="D12" s="129"/>
-      <c r="E12" s="130"/>
+      <c r="C12" s="127"/>
+      <c r="D12" s="127"/>
+      <c r="E12" s="128"/>
       <c r="F12" s="71">
         <f>SUM(F3:F10)</f>
         <v>17</v>
@@ -7619,7 +7618,7 @@
       </c>
     </row>
     <row r="13" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="123">
+      <c r="A13" s="120">
         <v>3</v>
       </c>
       <c r="B13" s="17" t="s">
@@ -7643,7 +7642,7 @@
       </c>
     </row>
     <row r="14" spans="1:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="123"/>
+      <c r="A14" s="120"/>
       <c r="B14" s="17" t="s">
         <v>40</v>
       </c>
@@ -7665,7 +7664,7 @@
       </c>
     </row>
     <row r="15" spans="1:7" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="123"/>
+      <c r="A15" s="120"/>
       <c r="B15" s="88" t="s">
         <v>46</v>
       </c>
@@ -7687,7 +7686,7 @@
       </c>
     </row>
     <row r="16" spans="1:7" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="131"/>
+      <c r="A16" s="129"/>
       <c r="B16" s="89" t="s">
         <v>277</v>
       </c>
@@ -7707,13 +7706,13 @@
       <c r="G16" s="22"/>
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A17" s="123"/>
-      <c r="B17" s="128" t="s">
+      <c r="A17" s="120"/>
+      <c r="B17" s="126" t="s">
         <v>41</v>
       </c>
-      <c r="C17" s="129"/>
-      <c r="D17" s="129"/>
-      <c r="E17" s="130"/>
+      <c r="C17" s="127"/>
+      <c r="D17" s="127"/>
+      <c r="E17" s="128"/>
       <c r="F17" s="71">
         <f>SUM(F13:F15)</f>
         <v>12</v>
@@ -7721,7 +7720,7 @@
       <c r="G17" s="63"/>
     </row>
     <row r="18" spans="1:18" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="118">
+      <c r="A18" s="115">
         <v>6</v>
       </c>
       <c r="B18" s="94" t="s">
@@ -7748,7 +7747,7 @@
       </c>
     </row>
     <row r="19" spans="1:18" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="120"/>
+      <c r="A19" s="117"/>
       <c r="B19" s="95" t="s">
         <v>277</v>
       </c>
@@ -7768,13 +7767,13 @@
       <c r="G19" s="22"/>
     </row>
     <row r="20" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A20" s="118"/>
-      <c r="B20" s="132" t="s">
+      <c r="A20" s="115"/>
+      <c r="B20" s="124" t="s">
         <v>84</v>
       </c>
-      <c r="C20" s="132"/>
-      <c r="D20" s="132"/>
-      <c r="E20" s="132"/>
+      <c r="C20" s="124"/>
+      <c r="D20" s="124"/>
+      <c r="E20" s="124"/>
       <c r="F20" s="71">
         <f>SUM(F18)</f>
         <v>34</v>
@@ -7789,7 +7788,7 @@
       <c r="M21" s="104"/>
     </row>
     <row r="22" spans="1:18" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="118">
+      <c r="A22" s="115">
         <v>7</v>
       </c>
       <c r="B22" s="94" t="s">
@@ -7811,24 +7810,24 @@
       <c r="G22" s="22" t="s">
         <v>68</v>
       </c>
-      <c r="I22" s="114" t="s">
+      <c r="I22" s="109" t="s">
         <v>25</v>
       </c>
-      <c r="J22" s="115" t="s">
+      <c r="J22" s="110" t="s">
         <v>289</v>
       </c>
-      <c r="K22" s="116" t="s">
+      <c r="K22" s="111" t="s">
         <v>290</v>
       </c>
-      <c r="L22" s="117" t="s">
+      <c r="L22" s="112" t="s">
         <v>291</v>
       </c>
-      <c r="M22" s="114" t="s">
+      <c r="M22" s="109" t="s">
         <v>276</v>
       </c>
     </row>
     <row r="23" spans="1:18" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="120"/>
+      <c r="A23" s="117"/>
       <c r="B23" s="95" t="s">
         <v>277</v>
       </c>
@@ -7846,10 +7845,10 @@
       </c>
       <c r="F23" s="74"/>
       <c r="G23" s="22"/>
-      <c r="I23" s="110">
+      <c r="I23" s="105">
         <v>2</v>
       </c>
-      <c r="J23" s="111">
+      <c r="J23" s="106">
         <f>C11</f>
         <v>12</v>
       </c>
@@ -7857,23 +7856,23 @@
         <f>D11</f>
         <v>5</v>
       </c>
-      <c r="L23" s="112">
+      <c r="L23" s="107">
         <f>E11</f>
         <v>0</v>
       </c>
-      <c r="M23" s="113">
+      <c r="M23" s="108">
         <f>F12</f>
         <v>17</v>
       </c>
     </row>
     <row r="24" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A24" s="118"/>
-      <c r="B24" s="132" t="s">
+      <c r="A24" s="115"/>
+      <c r="B24" s="124" t="s">
         <v>278</v>
       </c>
-      <c r="C24" s="132"/>
-      <c r="D24" s="132"/>
-      <c r="E24" s="132"/>
+      <c r="C24" s="124"/>
+      <c r="D24" s="124"/>
+      <c r="E24" s="124"/>
       <c r="F24" s="71">
         <f>SUM(F22)</f>
         <v>23</v>
@@ -7938,7 +7937,7 @@
       <c r="R25" s="97"/>
     </row>
     <row r="26" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="118">
+      <c r="A26" s="115">
         <v>8</v>
       </c>
       <c r="B26" s="25" t="s">
@@ -7986,7 +7985,7 @@
       <c r="R26" s="97"/>
     </row>
     <row r="27" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A27" s="118"/>
+      <c r="A27" s="115"/>
       <c r="B27" s="25" t="s">
         <v>206</v>
       </c>
@@ -8031,8 +8030,8 @@
       <c r="Q27" s="97"/>
       <c r="R27" s="97"/>
     </row>
-    <row r="28" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="118"/>
+    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A28" s="115"/>
       <c r="B28" s="25" t="s">
         <v>277</v>
       </c>
@@ -8075,59 +8074,59 @@
       <c r="Q28" s="97"/>
       <c r="R28" s="97"/>
     </row>
-    <row r="29" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="118"/>
-      <c r="B29" s="118" t="s">
+    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A29" s="115"/>
+      <c r="B29" s="115" t="s">
         <v>279</v>
       </c>
-      <c r="C29" s="118"/>
-      <c r="D29" s="118"/>
-      <c r="E29" s="118"/>
+      <c r="C29" s="115"/>
+      <c r="D29" s="115"/>
+      <c r="E29" s="115"/>
       <c r="F29" s="71">
         <f>SUM(F26:F27)</f>
         <v>25</v>
       </c>
       <c r="G29" s="63"/>
-      <c r="I29" s="105">
+      <c r="I29" s="130">
         <v>10</v>
       </c>
-      <c r="J29" s="106">
+      <c r="J29" s="4">
         <f>C39</f>
         <v>9</v>
       </c>
-      <c r="K29" s="107">
+      <c r="K29" s="4">
         <f>D39</f>
         <v>5</v>
       </c>
-      <c r="L29" s="108">
+      <c r="L29" s="4">
         <f>E39</f>
         <v>0</v>
       </c>
-      <c r="M29" s="109">
+      <c r="M29" s="4">
         <f t="shared" si="2"/>
         <v>14</v>
       </c>
     </row>
     <row r="30" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="I30" s="92">
+      <c r="I30" s="130">
         <v>11</v>
       </c>
-      <c r="J30" s="91">
+      <c r="J30" s="4">
         <v>4</v>
       </c>
       <c r="K30" s="4">
         <v>10</v>
       </c>
-      <c r="L30" s="90">
+      <c r="L30" s="4">
         <v>10</v>
       </c>
-      <c r="M30" s="73">
+      <c r="M30" s="4">
         <f t="shared" si="2"/>
         <v>24</v>
       </c>
     </row>
-    <row r="31" spans="1:18" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="118">
+    <row r="31" spans="1:18" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="115">
         <v>9</v>
       </c>
       <c r="B31" s="25" t="s">
@@ -8149,26 +8148,26 @@
       <c r="G31" s="22" t="s">
         <v>68</v>
       </c>
-      <c r="I31" s="98">
+      <c r="I31" s="130">
         <v>12</v>
       </c>
-      <c r="J31" s="99">
-        <v>5</v>
-      </c>
-      <c r="K31" s="100">
-        <v>5</v>
-      </c>
-      <c r="L31" s="101">
+      <c r="J31" s="4">
+        <v>5</v>
+      </c>
+      <c r="K31" s="4">
+        <v>5</v>
+      </c>
+      <c r="L31" s="4">
         <f>E36</f>
         <v>0</v>
       </c>
-      <c r="M31" s="102">
+      <c r="M31" s="4">
         <f t="shared" si="2"/>
         <v>10</v>
       </c>
     </row>
-    <row r="32" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="118"/>
+    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A32" s="115"/>
       <c r="B32" s="25" t="s">
         <v>284</v>
       </c>
@@ -8184,26 +8183,23 @@
         <v>2</v>
       </c>
       <c r="G32" s="22"/>
-      <c r="I32" s="105">
+      <c r="I32" s="130">
         <v>13</v>
       </c>
-      <c r="J32" s="106">
+      <c r="J32" s="4">
         <v>8</v>
       </c>
-      <c r="K32" s="107">
-        <v>5</v>
-      </c>
-      <c r="L32" s="108">
-        <f>E42</f>
-        <v>0</v>
-      </c>
-      <c r="M32" s="109">
+      <c r="K32" s="4">
+        <v>5</v>
+      </c>
+      <c r="L32" s="4"/>
+      <c r="M32" s="4">
         <f t="shared" si="2"/>
         <v>13</v>
       </c>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A33" s="118"/>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A33" s="115"/>
       <c r="B33" s="25" t="s">
         <v>277</v>
       </c>
@@ -8222,35 +8218,38 @@
       <c r="G33" s="64" t="s">
         <v>24</v>
       </c>
-      <c r="I33" s="133">
+      <c r="I33" s="130">
         <v>14</v>
       </c>
-      <c r="J33">
-        <v>5</v>
-      </c>
-      <c r="K33">
-        <v>5</v>
-      </c>
-      <c r="L33">
+      <c r="J33" s="4">
+        <v>5</v>
+      </c>
+      <c r="K33" s="4">
+        <v>5</v>
+      </c>
+      <c r="L33" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A34" s="118"/>
-      <c r="B34" s="118" t="s">
+      <c r="M33" s="4">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A34" s="115"/>
+      <c r="B34" s="115" t="s">
         <v>280</v>
       </c>
-      <c r="C34" s="118"/>
-      <c r="D34" s="118"/>
-      <c r="E34" s="118"/>
+      <c r="C34" s="115"/>
+      <c r="D34" s="115"/>
+      <c r="E34" s="115"/>
       <c r="F34" s="71">
         <f>SUM(F31:F33)</f>
         <v>9</v>
       </c>
       <c r="G34" s="63"/>
     </row>
-    <row r="36" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="118">
+    <row r="36" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="115">
         <v>10</v>
       </c>
       <c r="B36" s="25" t="s">
@@ -8273,8 +8272,8 @@
         <v>68</v>
       </c>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A37" s="118"/>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A37" s="115"/>
       <c r="B37" s="25" t="s">
         <v>287</v>
       </c>
@@ -8295,8 +8294,8 @@
         <v>24</v>
       </c>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A38" s="118"/>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A38" s="115"/>
       <c r="B38" s="25" t="s">
         <v>288</v>
       </c>
@@ -8315,8 +8314,8 @@
       </c>
       <c r="G38" s="64"/>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A39" s="118"/>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A39" s="115"/>
       <c r="B39" s="25" t="s">
         <v>285</v>
       </c>
@@ -8335,22 +8334,436 @@
       <c r="F39" s="64"/>
       <c r="G39" s="64"/>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A40" s="118"/>
-      <c r="B40" s="118" t="s">
+    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A40" s="115"/>
+      <c r="B40" s="115" t="s">
         <v>281</v>
       </c>
-      <c r="C40" s="118"/>
-      <c r="D40" s="118"/>
-      <c r="E40" s="118"/>
+      <c r="C40" s="115"/>
+      <c r="D40" s="115"/>
+      <c r="E40" s="115"/>
       <c r="F40" s="71">
         <f>SUM(F36:F39)</f>
         <v>14</v>
       </c>
       <c r="G40" s="63"/>
     </row>
+    <row r="43" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+      <c r="A43" s="115">
+        <v>11</v>
+      </c>
+      <c r="B43" s="25" t="s">
+        <v>286</v>
+      </c>
+      <c r="C43" s="114">
+        <v>1</v>
+      </c>
+      <c r="D43" s="114">
+        <v>0</v>
+      </c>
+      <c r="E43" s="24">
+        <v>0</v>
+      </c>
+      <c r="F43" s="114">
+        <f>SUM(C43,D43*5,E43*10)</f>
+        <v>1</v>
+      </c>
+      <c r="G43" s="22" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A44" s="115"/>
+      <c r="B44" s="25" t="s">
+        <v>287</v>
+      </c>
+      <c r="C44" s="114">
+        <v>2</v>
+      </c>
+      <c r="D44" s="114">
+        <v>1</v>
+      </c>
+      <c r="E44" s="24">
+        <v>0</v>
+      </c>
+      <c r="F44" s="114">
+        <f t="shared" ref="F44:F45" si="5">SUM(C44,D44*5,E44*10)</f>
+        <v>7</v>
+      </c>
+      <c r="G44" s="114" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A45" s="115"/>
+      <c r="B45" s="25" t="s">
+        <v>288</v>
+      </c>
+      <c r="C45" s="114">
+        <v>1</v>
+      </c>
+      <c r="D45" s="114">
+        <v>1</v>
+      </c>
+      <c r="E45" s="24">
+        <v>1</v>
+      </c>
+      <c r="F45" s="114">
+        <f t="shared" si="5"/>
+        <v>16</v>
+      </c>
+      <c r="G45" s="114"/>
+    </row>
+    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A46" s="115"/>
+      <c r="B46" s="25" t="s">
+        <v>285</v>
+      </c>
+      <c r="C46" s="114">
+        <f>SUM(C43:C45)</f>
+        <v>4</v>
+      </c>
+      <c r="D46" s="114">
+        <f>SUM(D43:D45)*5</f>
+        <v>10</v>
+      </c>
+      <c r="E46" s="24">
+        <f>SUM(E43:E45)*10</f>
+        <v>10</v>
+      </c>
+      <c r="F46" s="114"/>
+      <c r="G46" s="114"/>
+    </row>
+    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A47" s="115"/>
+      <c r="B47" s="115" t="s">
+        <v>292</v>
+      </c>
+      <c r="C47" s="115"/>
+      <c r="D47" s="115"/>
+      <c r="E47" s="115"/>
+      <c r="F47" s="71">
+        <f>SUM(F43:F46)</f>
+        <v>24</v>
+      </c>
+      <c r="G47" s="113"/>
+    </row>
+    <row r="49" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A49" s="115">
+        <v>12</v>
+      </c>
+      <c r="B49" s="25" t="s">
+        <v>295</v>
+      </c>
+      <c r="C49" s="114">
+        <v>1</v>
+      </c>
+      <c r="D49" s="114">
+        <v>0</v>
+      </c>
+      <c r="E49" s="24">
+        <v>0</v>
+      </c>
+      <c r="F49" s="114">
+        <f>SUM(C49,D49*5,E49*10)</f>
+        <v>1</v>
+      </c>
+      <c r="G49" s="22" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A50" s="115"/>
+      <c r="B50" s="25" t="s">
+        <v>293</v>
+      </c>
+      <c r="C50" s="114">
+        <v>2</v>
+      </c>
+      <c r="D50" s="114">
+        <v>0</v>
+      </c>
+      <c r="E50" s="24">
+        <v>0</v>
+      </c>
+      <c r="F50" s="114">
+        <f t="shared" ref="F50:F51" si="6">SUM(C50,D50*5,E50*10)</f>
+        <v>2</v>
+      </c>
+      <c r="G50" s="114" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A51" s="115"/>
+      <c r="B51" s="25" t="s">
+        <v>288</v>
+      </c>
+      <c r="C51" s="114">
+        <v>2</v>
+      </c>
+      <c r="D51" s="114">
+        <v>1</v>
+      </c>
+      <c r="E51" s="24">
+        <v>0</v>
+      </c>
+      <c r="F51" s="114">
+        <f t="shared" si="6"/>
+        <v>7</v>
+      </c>
+      <c r="G51" s="114"/>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A52" s="115"/>
+      <c r="B52" s="25" t="s">
+        <v>285</v>
+      </c>
+      <c r="C52" s="114">
+        <f>SUM(C49:C51)</f>
+        <v>5</v>
+      </c>
+      <c r="D52" s="114">
+        <f>SUM(D49:D51)*5</f>
+        <v>5</v>
+      </c>
+      <c r="E52" s="24">
+        <f>SUM(E49:E51)*10</f>
+        <v>0</v>
+      </c>
+      <c r="F52" s="114"/>
+      <c r="G52" s="114"/>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A53" s="115"/>
+      <c r="B53" s="115" t="s">
+        <v>281</v>
+      </c>
+      <c r="C53" s="115"/>
+      <c r="D53" s="115"/>
+      <c r="E53" s="115"/>
+      <c r="F53" s="71">
+        <f>SUM(F49:F52)</f>
+        <v>10</v>
+      </c>
+      <c r="G53" s="113"/>
+    </row>
+    <row r="55" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A55" s="115">
+        <v>13</v>
+      </c>
+      <c r="B55" s="25" t="s">
+        <v>294</v>
+      </c>
+      <c r="C55" s="114">
+        <v>3</v>
+      </c>
+      <c r="D55" s="114">
+        <v>0</v>
+      </c>
+      <c r="E55" s="24">
+        <v>0</v>
+      </c>
+      <c r="F55" s="114">
+        <f>SUM(C55,D55*5,E55*10)</f>
+        <v>3</v>
+      </c>
+      <c r="G55" s="22" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A56" s="115"/>
+      <c r="B56" s="25" t="s">
+        <v>287</v>
+      </c>
+      <c r="C56" s="114">
+        <v>3</v>
+      </c>
+      <c r="D56" s="114">
+        <v>0</v>
+      </c>
+      <c r="E56" s="24">
+        <v>0</v>
+      </c>
+      <c r="F56" s="114">
+        <f t="shared" ref="F56:F57" si="7">SUM(C56,D56*5,E56*10)</f>
+        <v>3</v>
+      </c>
+      <c r="G56" s="114" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A57" s="115"/>
+      <c r="B57" s="25" t="s">
+        <v>293</v>
+      </c>
+      <c r="C57" s="114">
+        <v>2</v>
+      </c>
+      <c r="D57" s="114">
+        <v>1</v>
+      </c>
+      <c r="E57" s="24">
+        <v>0</v>
+      </c>
+      <c r="F57" s="114">
+        <f t="shared" si="7"/>
+        <v>7</v>
+      </c>
+      <c r="G57" s="114"/>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A58" s="115"/>
+      <c r="B58" s="25" t="s">
+        <v>285</v>
+      </c>
+      <c r="C58" s="114">
+        <f>SUM(C55:C57)</f>
+        <v>8</v>
+      </c>
+      <c r="D58" s="114">
+        <f>SUM(D55:D57)*5</f>
+        <v>5</v>
+      </c>
+      <c r="E58" s="24">
+        <f>SUM(E55:E57)*10</f>
+        <v>0</v>
+      </c>
+      <c r="F58" s="114"/>
+      <c r="G58" s="114"/>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A59" s="115"/>
+      <c r="B59" s="115" t="s">
+        <v>281</v>
+      </c>
+      <c r="C59" s="115"/>
+      <c r="D59" s="115"/>
+      <c r="E59" s="115"/>
+      <c r="F59" s="71">
+        <f>SUM(F55:F58)</f>
+        <v>13</v>
+      </c>
+      <c r="G59" s="113"/>
+    </row>
+    <row r="61" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A61" s="115">
+        <v>14</v>
+      </c>
+      <c r="B61" s="25" t="s">
+        <v>294</v>
+      </c>
+      <c r="C61" s="114">
+        <v>1</v>
+      </c>
+      <c r="D61" s="114">
+        <v>0</v>
+      </c>
+      <c r="E61" s="24">
+        <v>0</v>
+      </c>
+      <c r="F61" s="114">
+        <f>SUM(C61,D61*5,E61*10)</f>
+        <v>1</v>
+      </c>
+      <c r="G61" s="22" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A62" s="115"/>
+      <c r="B62" s="25" t="s">
+        <v>287</v>
+      </c>
+      <c r="C62" s="114">
+        <v>2</v>
+      </c>
+      <c r="D62" s="114">
+        <v>0</v>
+      </c>
+      <c r="E62" s="24">
+        <v>0</v>
+      </c>
+      <c r="F62" s="114">
+        <f t="shared" ref="F62:F63" si="8">SUM(C62,D62*5,E62*10)</f>
+        <v>2</v>
+      </c>
+      <c r="G62" s="114" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A63" s="115"/>
+      <c r="B63" s="25" t="s">
+        <v>293</v>
+      </c>
+      <c r="C63" s="114">
+        <v>2</v>
+      </c>
+      <c r="D63" s="114">
+        <v>1</v>
+      </c>
+      <c r="E63" s="24">
+        <v>0</v>
+      </c>
+      <c r="F63" s="114">
+        <f t="shared" si="8"/>
+        <v>7</v>
+      </c>
+      <c r="G63" s="114"/>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A64" s="115"/>
+      <c r="B64" s="25" t="s">
+        <v>285</v>
+      </c>
+      <c r="C64" s="114">
+        <f>SUM(C61:C63)</f>
+        <v>5</v>
+      </c>
+      <c r="D64" s="114">
+        <f>SUM(D61:D63)*5</f>
+        <v>5</v>
+      </c>
+      <c r="E64" s="24">
+        <f>SUM(E61:E63)*10</f>
+        <v>0</v>
+      </c>
+      <c r="F64" s="114"/>
+      <c r="G64" s="114"/>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A65" s="115"/>
+      <c r="B65" s="115" t="s">
+        <v>281</v>
+      </c>
+      <c r="C65" s="115"/>
+      <c r="D65" s="115"/>
+      <c r="E65" s="115"/>
+      <c r="F65" s="71">
+        <f>SUM(F61:F64)</f>
+        <v>10</v>
+      </c>
+      <c r="G65" s="113"/>
+    </row>
   </sheetData>
-  <mergeCells count="14">
+  <mergeCells count="22">
+    <mergeCell ref="A55:A59"/>
+    <mergeCell ref="B59:E59"/>
+    <mergeCell ref="A61:A65"/>
+    <mergeCell ref="B65:E65"/>
+    <mergeCell ref="A43:A47"/>
+    <mergeCell ref="B47:E47"/>
+    <mergeCell ref="A49:A53"/>
+    <mergeCell ref="B53:E53"/>
+    <mergeCell ref="A3:A12"/>
+    <mergeCell ref="B12:E12"/>
+    <mergeCell ref="A13:A17"/>
+    <mergeCell ref="B17:E17"/>
+    <mergeCell ref="A18:A20"/>
+    <mergeCell ref="B20:E20"/>
     <mergeCell ref="A36:A40"/>
     <mergeCell ref="B40:E40"/>
     <mergeCell ref="A22:A24"/>
@@ -8359,12 +8772,6 @@
     <mergeCell ref="B29:E29"/>
     <mergeCell ref="A31:A34"/>
     <mergeCell ref="B34:E34"/>
-    <mergeCell ref="A3:A12"/>
-    <mergeCell ref="B12:E12"/>
-    <mergeCell ref="A13:A17"/>
-    <mergeCell ref="B17:E17"/>
-    <mergeCell ref="A18:A20"/>
-    <mergeCell ref="B20:E20"/>
   </mergeCells>
   <conditionalFormatting sqref="C3:E9 C11:E11 D10:E10">
     <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">

</xml_diff>